<commit_message>
updates to Norwegian Data
</commit_message>
<xml_diff>
--- a/in_s_NO_1950_2007_cl_statbank.xlsx
+++ b/in_s_NO_1950_2007_cl_statbank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/ericyo_ntnu_no/Documents/VehicleFleetDatabase/vehicle_fleet_git_hub/vehicle_stock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F8DAB2F-57D6-584F-A107-BEA1524AA83A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{5F8DAB2F-57D6-584F-A107-BEA1524AA83A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A1885B9A-4499-114A-B22A-C58FF635592F}"/>
   <bookViews>
     <workbookView xWindow="7040" yWindow="460" windowWidth="21760" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="108">
   <si>
     <t>01960: Registered vehicles, by contents and year</t>
   </si>
@@ -394,6 +394,9 @@
   </si>
   <si>
     <t>https://www.ssb.no/en/statbank/table/01960/</t>
+  </si>
+  <si>
+    <t>class</t>
   </si>
 </sst>
 </file>
@@ -780,7 +783,7 @@
   <dimension ref="A1:BG11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -792,6 +795,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>107</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>

</xml_diff>